<commit_message>
Update Diwali Sales Data_xLOOKUP(best LOOKUP)_multiple_columns_slicing.xlsx
INDEX AND MATCH ADDED HERE
</commit_message>
<xml_diff>
--- a/Lookups/Diwali Sales Data_xLOOKUP(best LOOKUP)_multiple_columns_slicing.xlsx
+++ b/Lookups/Diwali Sales Data_xLOOKUP(best LOOKUP)_multiple_columns_slicing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Excel-For-Data-Analysis\Lookups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F266361-7C49-49EA-9155-816F3A55F3AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7CBB26-9C78-404B-896D-69DF02628FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{15B3E89B-59B3-48C2-BDF8-FE836FD70981}"/>
   </bookViews>
@@ -43,6 +43,7 @@
   <authors>
     <author>tc={71DDC270-3DFC-4488-9891-E920FCA9649F}</author>
     <author>tc={1A4C8D45-B124-48B8-961A-0D476A3A1730}</author>
+    <author>tc={AA977669-C33C-434E-844C-CDDC8ABA7DE4}</author>
   </authors>
   <commentList>
     <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{71DDC270-3DFC-4488-9891-E920FCA9649F}">
@@ -64,12 +65,20 @@
 f3 click for find column name </t>
       </text>
     </comment>
+    <comment ref="L17" authorId="2" shapeId="0" xr:uid="{AA977669-C33C-434E-844C-CDDC8ABA7DE4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    =INDEX(B:B,MATCH(M4,B:B,0))</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -91,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="137">
   <si>
     <t>User_ID</t>
   </si>
@@ -499,6 +508,9 @@
   </si>
   <si>
     <t>NOTE</t>
+  </si>
+  <si>
+    <t>INDEX</t>
   </si>
 </sst>
 </file>
@@ -641,12 +653,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1" tint="4.9989318521683403E-2"/>
@@ -654,8 +660,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -856,6 +868,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1068,18 +1086,20 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1467,6 +1487,9 @@
     <text xml:space="preserve">=XLOOKUP(L4,User_ID,Cust_name :State, "Not Found",0,1)
 f3 click for find column name </text>
   </threadedComment>
+  <threadedComment ref="L17" dT="2024-06-19T17:48:57.43" personId="{65FE81FC-66D5-49B9-B935-0E2A63D7F1A6}" id="{AA977669-C33C-434E-844C-CDDC8ABA7DE4}">
+    <text>=INDEX(B:B,MATCH(M4,B:B,0))</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -1475,7 +1498,7 @@
   <dimension ref="A1:Q101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1517,13 +1540,13 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
@@ -1550,12 +1573,12 @@
       <c r="H2">
         <v>23952</v>
       </c>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="6" t="s">
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="5" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2101,7 +2124,7 @@
         <v>23518</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1001505</v>
       </c>
@@ -2126,8 +2149,12 @@
       <c r="H17">
         <v>23515</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L17" s="7" t="str">
+        <f>INDEX(B:B,MATCH(M4,B:B,0))</f>
+        <v>Sanskriti</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1000900</v>
       </c>
@@ -2152,8 +2179,11 @@
       <c r="H18">
         <v>23513</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L18" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1005908</v>
       </c>
@@ -2179,7 +2209,7 @@
         <v>23462</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1001101</v>
       </c>
@@ -2205,7 +2235,7 @@
         <v>23456</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1004736</v>
       </c>
@@ -2231,7 +2261,7 @@
         <v>23451</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1004037</v>
       </c>
@@ -2257,7 +2287,7 @@
         <v>23434</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1002340</v>
       </c>
@@ -2283,7 +2313,7 @@
         <v>23389</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1005664</v>
       </c>
@@ -2309,7 +2339,7 @@
         <v>23365</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1002523</v>
       </c>
@@ -2335,7 +2365,7 @@
         <v>23326</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1002503</v>
       </c>
@@ -2361,7 +2391,7 @@
         <v>23314</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>1002638</v>
       </c>
@@ -2387,7 +2417,7 @@
         <v>23306</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1004505</v>
       </c>
@@ -2413,7 +2443,7 @@
         <v>23302</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1004957</v>
       </c>
@@ -2439,7 +2469,7 @@
         <v>23285</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1005649</v>
       </c>
@@ -2465,7 +2495,7 @@
         <v>23281</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1004508</v>
       </c>
@@ -2491,7 +2521,7 @@
         <v>23270</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1002520</v>
       </c>

</xml_diff>